<commit_message>
start customer_page + correct info's location about items
</commit_message>
<xml_diff>
--- a/src/main/resources/database/item.xlsx
+++ b/src/main/resources/database/item.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaIDE\test\src\main\resources\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\clothing-store\src\main\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B646140-4C55-4E4F-9840-6AC66AC6A8D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C5277-0220-4258-B4B6-703217DACA9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6372" yWindow="2484" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="173">
   <si>
     <t>4.99 $</t>
-  </si>
-  <si>
-    <t>shop</t>
   </si>
   <si>
     <t>item1.png</t>
@@ -872,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,15 +883,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1">
         <v>1</v>
       </c>
     </row>
@@ -903,15 +900,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
@@ -920,15 +917,15 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
     </row>
@@ -937,15 +934,15 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E4">
         <v>1</v>
       </c>
     </row>
@@ -954,15 +951,15 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
     </row>
@@ -971,15 +968,15 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
     </row>
@@ -988,15 +985,15 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
         <v>82</v>
       </c>
-      <c r="D7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="E7">
         <v>1</v>
       </c>
     </row>
@@ -1005,15 +1002,15 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8">
         <v>1</v>
       </c>
     </row>
@@ -1022,15 +1019,15 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
     </row>
@@ -1039,15 +1036,15 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
         <v>1</v>
       </c>
     </row>
@@ -1056,15 +1053,15 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
         <v>1</v>
       </c>
     </row>
@@ -1073,15 +1070,15 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12">
         <v>1</v>
       </c>
     </row>
@@ -1090,15 +1087,15 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
     </row>
@@ -1107,15 +1104,15 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14">
         <v>1</v>
       </c>
     </row>
@@ -1124,15 +1121,15 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15">
         <v>1</v>
       </c>
     </row>
@@ -1141,15 +1138,15 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
         <v>1</v>
       </c>
     </row>
@@ -1158,15 +1155,15 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17">
         <v>1</v>
       </c>
     </row>
@@ -1175,15 +1172,15 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
     </row>
@@ -1192,15 +1189,15 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19">
         <v>1</v>
       </c>
     </row>
@@ -1209,15 +1206,15 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
     </row>
@@ -1226,15 +1223,15 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
       <c r="D21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21">
         <v>1</v>
       </c>
     </row>
@@ -1243,15 +1240,15 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22">
         <v>1</v>
       </c>
     </row>
@@ -1260,15 +1257,15 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23">
         <v>1</v>
       </c>
     </row>
@@ -1278,15 +1275,15 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24">
         <v>1</v>
       </c>
     </row>
@@ -1296,15 +1293,15 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25">
         <v>1</v>
       </c>
     </row>
@@ -1314,15 +1311,15 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26">
         <v>1</v>
       </c>
     </row>
@@ -1332,15 +1329,15 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27">
         <v>1</v>
       </c>
     </row>
@@ -1350,15 +1347,15 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28">
         <v>1</v>
       </c>
     </row>
@@ -1368,15 +1365,15 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29">
         <v>1</v>
       </c>
     </row>
@@ -1386,15 +1383,15 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
         <v>93</v>
       </c>
-      <c r="D30" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="E30">
         <v>1</v>
       </c>
     </row>
@@ -1404,15 +1401,15 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
         <v>93</v>
       </c>
-      <c r="D31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="E31">
         <v>1</v>
       </c>
     </row>
@@ -1422,15 +1419,15 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32">
         <v>1</v>
       </c>
     </row>
@@ -1440,15 +1437,15 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33">
         <v>1</v>
       </c>
     </row>
@@ -1458,15 +1455,15 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34">
         <v>1</v>
       </c>
     </row>
@@ -1476,15 +1473,15 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35">
         <v>1</v>
       </c>
     </row>
@@ -1494,15 +1491,15 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36">
         <v>1</v>
       </c>
     </row>
@@ -1512,15 +1509,15 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37">
         <v>1</v>
       </c>
     </row>
@@ -1530,15 +1527,15 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38">
         <v>1</v>
       </c>
     </row>
@@ -1548,15 +1545,15 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
-      </c>
-      <c r="E39" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39">
         <v>1</v>
       </c>
     </row>
@@ -1566,15 +1563,15 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40">
         <v>1</v>
       </c>
     </row>
@@ -1584,15 +1581,15 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41">
         <v>1</v>
       </c>
     </row>
@@ -1602,15 +1599,15 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D42" t="s">
-        <v>108</v>
-      </c>
-      <c r="E42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42">
         <v>1</v>
       </c>
     </row>
@@ -1620,15 +1617,15 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" t="s">
+        <v>79</v>
+      </c>
+      <c r="E43">
         <v>1</v>
       </c>
     </row>
@@ -1638,15 +1635,15 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>107</v>
-      </c>
-      <c r="E44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44">
         <v>1</v>
       </c>
     </row>
@@ -1656,15 +1653,15 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D45" t="s">
         <v>0</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45">
         <v>1</v>
       </c>
     </row>
@@ -1674,15 +1671,15 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" t="s">
         <v>105</v>
       </c>
-      <c r="D46" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="E46">
         <v>1</v>
       </c>
     </row>
@@ -1692,15 +1689,15 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" t="s">
+        <v>108</v>
+      </c>
+      <c r="E47">
         <v>1</v>
       </c>
     </row>
@@ -1710,15 +1707,15 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>101</v>
-      </c>
-      <c r="E48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48">
         <v>1</v>
       </c>
     </row>
@@ -1728,15 +1725,15 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D49" t="s">
         <v>0</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49">
         <v>1</v>
       </c>
     </row>
@@ -1746,15 +1743,15 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D50" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50">
         <v>1</v>
       </c>
     </row>
@@ -1764,15 +1761,15 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>101</v>
-      </c>
-      <c r="E51" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51">
         <v>1</v>
       </c>
     </row>
@@ -1782,15 +1779,15 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>104</v>
-      </c>
-      <c r="E52" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52">
         <v>1</v>
       </c>
     </row>
@@ -1800,15 +1797,15 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>103</v>
-      </c>
-      <c r="E53" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53">
         <v>1</v>
       </c>
     </row>
@@ -1818,15 +1815,15 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>104</v>
-      </c>
-      <c r="E54" t="s">
+        <v>103</v>
+      </c>
+      <c r="E54">
         <v>1</v>
       </c>
     </row>
@@ -1836,15 +1833,15 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D55" t="s">
-        <v>104</v>
-      </c>
-      <c r="E55" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55">
         <v>1</v>
       </c>
     </row>
@@ -1854,15 +1851,15 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D56" t="s">
-        <v>110</v>
-      </c>
-      <c r="E56" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56">
         <v>1</v>
       </c>
     </row>
@@ -1872,15 +1869,15 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D57" t="s">
-        <v>103</v>
-      </c>
-      <c r="E57" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57">
         <v>1</v>
       </c>
     </row>
@@ -1890,15 +1887,15 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D58" t="s">
-        <v>103</v>
-      </c>
-      <c r="E58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E58">
         <v>1</v>
       </c>
     </row>
@@ -1908,15 +1905,15 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D59" t="s">
-        <v>103</v>
-      </c>
-      <c r="E59" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59">
         <v>1</v>
       </c>
     </row>
@@ -1926,15 +1923,15 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D60" t="s">
-        <v>94</v>
-      </c>
-      <c r="E60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E60">
         <v>1</v>
       </c>
     </row>
@@ -1944,15 +1941,15 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D61" t="s">
-        <v>102</v>
-      </c>
-      <c r="E61" t="s">
+        <v>101</v>
+      </c>
+      <c r="E61">
         <v>1</v>
       </c>
     </row>
@@ -1962,15 +1959,15 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D62" t="s">
-        <v>101</v>
-      </c>
-      <c r="E62" t="s">
+        <v>100</v>
+      </c>
+      <c r="E62">
         <v>1</v>
       </c>
     </row>
@@ -1980,15 +1977,15 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>95</v>
-      </c>
-      <c r="E63" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63">
         <v>1</v>
       </c>
     </row>
@@ -1998,15 +1995,15 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D64" t="s">
-        <v>90</v>
-      </c>
-      <c r="E64" t="s">
+        <v>89</v>
+      </c>
+      <c r="E64">
         <v>1</v>
       </c>
     </row>
@@ -2016,15 +2013,15 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D65" t="s">
-        <v>103</v>
-      </c>
-      <c r="E65" t="s">
+        <v>102</v>
+      </c>
+      <c r="E65">
         <v>1</v>
       </c>
     </row>
@@ -2034,15 +2031,15 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D66" t="s">
-        <v>104</v>
-      </c>
-      <c r="E66" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66">
         <v>1</v>
       </c>
     </row>
@@ -2052,15 +2049,15 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D67" t="s">
-        <v>103</v>
-      </c>
-      <c r="E67" t="s">
+        <v>102</v>
+      </c>
+      <c r="E67">
         <v>1</v>
       </c>
     </row>
@@ -2070,15 +2067,15 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D68" t="s">
-        <v>111</v>
-      </c>
-      <c r="E68" t="s">
+        <v>110</v>
+      </c>
+      <c r="E68">
         <v>1</v>
       </c>
     </row>
@@ -2088,15 +2085,15 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D69" t="s">
-        <v>112</v>
-      </c>
-      <c r="E69" t="s">
+        <v>111</v>
+      </c>
+      <c r="E69">
         <v>1</v>
       </c>
     </row>
@@ -2106,15 +2103,15 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D70" t="s">
-        <v>94</v>
-      </c>
-      <c r="E70" t="s">
+        <v>93</v>
+      </c>
+      <c r="E70">
         <v>1</v>
       </c>
     </row>
@@ -2124,15 +2121,15 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D71" t="s">
-        <v>97</v>
-      </c>
-      <c r="E71" t="s">
+        <v>96</v>
+      </c>
+      <c r="E71">
         <v>1</v>
       </c>
     </row>
@@ -2142,15 +2139,15 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D72" t="s">
-        <v>96</v>
-      </c>
-      <c r="E72" t="s">
+        <v>95</v>
+      </c>
+      <c r="E72">
         <v>1</v>
       </c>
     </row>
@@ -2160,15 +2157,15 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C73" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D73" t="s">
-        <v>172</v>
-      </c>
-      <c r="E73" t="s">
+        <v>171</v>
+      </c>
+      <c r="E73">
         <v>1</v>
       </c>
     </row>
@@ -2178,15 +2175,15 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D74" t="s">
-        <v>139</v>
-      </c>
-      <c r="E74" t="s">
+        <v>138</v>
+      </c>
+      <c r="E74">
         <v>1</v>
       </c>
     </row>
@@ -2196,15 +2193,15 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C75" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D75" t="s">
-        <v>139</v>
-      </c>
-      <c r="E75" t="s">
+        <v>138</v>
+      </c>
+      <c r="E75">
         <v>1</v>
       </c>
     </row>
@@ -2214,15 +2211,15 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C76" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D76" t="s">
-        <v>139</v>
-      </c>
-      <c r="E76" t="s">
+        <v>138</v>
+      </c>
+      <c r="E76">
         <v>1</v>
       </c>
     </row>
@@ -2232,15 +2229,15 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C77" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D77" t="s">
-        <v>139</v>
-      </c>
-      <c r="E77" t="s">
+        <v>138</v>
+      </c>
+      <c r="E77">
         <v>1</v>
       </c>
     </row>
@@ -2250,15 +2247,15 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C78" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D78" t="s">
-        <v>139</v>
-      </c>
-      <c r="E78" t="s">
+        <v>138</v>
+      </c>
+      <c r="E78">
         <v>1</v>
       </c>
     </row>
@@ -2268,15 +2265,15 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D79" t="s">
-        <v>139</v>
-      </c>
-      <c r="E79" t="s">
+        <v>138</v>
+      </c>
+      <c r="E79">
         <v>1</v>
       </c>
     </row>
@@ -2286,15 +2283,15 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C80" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D80" t="s">
-        <v>139</v>
-      </c>
-      <c r="E80" t="s">
+        <v>138</v>
+      </c>
+      <c r="E80">
         <v>1</v>
       </c>
     </row>
@@ -2304,15 +2301,15 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D81" t="s">
-        <v>139</v>
-      </c>
-      <c r="E81" t="s">
+        <v>138</v>
+      </c>
+      <c r="E81">
         <v>1</v>
       </c>
     </row>
@@ -2322,15 +2319,15 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C82" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D82" t="s">
-        <v>139</v>
-      </c>
-      <c r="E82" t="s">
+        <v>138</v>
+      </c>
+      <c r="E82">
         <v>1</v>
       </c>
     </row>
@@ -2340,15 +2337,15 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D83" t="s">
-        <v>139</v>
-      </c>
-      <c r="E83" t="s">
+        <v>138</v>
+      </c>
+      <c r="E83">
         <v>1</v>
       </c>
     </row>
@@ -2358,15 +2355,15 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D84" t="s">
-        <v>139</v>
-      </c>
-      <c r="E84" t="s">
+        <v>138</v>
+      </c>
+      <c r="E84">
         <v>1</v>
       </c>
     </row>
@@ -2376,15 +2373,15 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C85" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D85" t="s">
-        <v>139</v>
-      </c>
-      <c r="E85" t="s">
+        <v>138</v>
+      </c>
+      <c r="E85">
         <v>1</v>
       </c>
     </row>
@@ -2394,15 +2391,15 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D86" t="s">
-        <v>139</v>
-      </c>
-      <c r="E86" t="s">
+        <v>138</v>
+      </c>
+      <c r="E86">
         <v>1</v>
       </c>
     </row>
@@ -2412,15 +2409,15 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C87" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D87" t="s">
-        <v>139</v>
-      </c>
-      <c r="E87" t="s">
+        <v>138</v>
+      </c>
+      <c r="E87">
         <v>1</v>
       </c>
     </row>
@@ -2430,15 +2427,15 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C88" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D88" t="s">
-        <v>139</v>
-      </c>
-      <c r="E88" t="s">
+        <v>138</v>
+      </c>
+      <c r="E88">
         <v>1</v>
       </c>
     </row>
@@ -2448,15 +2445,15 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C89" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D89" t="s">
-        <v>139</v>
-      </c>
-      <c r="E89" t="s">
+        <v>138</v>
+      </c>
+      <c r="E89">
         <v>1</v>
       </c>
     </row>
@@ -2466,15 +2463,15 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C90" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D90" t="s">
-        <v>139</v>
-      </c>
-      <c r="E90" t="s">
+        <v>138</v>
+      </c>
+      <c r="E90">
         <v>1</v>
       </c>
     </row>
@@ -2484,15 +2481,15 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C91" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D91" t="s">
-        <v>139</v>
-      </c>
-      <c r="E91" t="s">
+        <v>138</v>
+      </c>
+      <c r="E91">
         <v>1</v>
       </c>
     </row>
@@ -2502,15 +2499,15 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D92" t="s">
-        <v>139</v>
-      </c>
-      <c r="E92" t="s">
+        <v>138</v>
+      </c>
+      <c r="E92">
         <v>1</v>
       </c>
     </row>
@@ -2520,15 +2517,15 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C93" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D93" t="s">
-        <v>139</v>
-      </c>
-      <c r="E93" t="s">
+        <v>138</v>
+      </c>
+      <c r="E93">
         <v>1</v>
       </c>
     </row>
@@ -2538,15 +2535,15 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C94" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D94" t="s">
-        <v>139</v>
-      </c>
-      <c r="E94" t="s">
+        <v>138</v>
+      </c>
+      <c r="E94">
         <v>1</v>
       </c>
     </row>
@@ -2556,15 +2553,15 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D95" t="s">
-        <v>139</v>
-      </c>
-      <c r="E95" t="s">
+        <v>138</v>
+      </c>
+      <c r="E95">
         <v>1</v>
       </c>
     </row>
@@ -2574,15 +2571,15 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C96" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D96" t="s">
-        <v>139</v>
-      </c>
-      <c r="E96" t="s">
+        <v>138</v>
+      </c>
+      <c r="E96">
         <v>1</v>
       </c>
     </row>
@@ -2592,15 +2589,15 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C97" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D97" t="s">
-        <v>139</v>
-      </c>
-      <c r="E97" t="s">
+        <v>138</v>
+      </c>
+      <c r="E97">
         <v>1</v>
       </c>
     </row>
@@ -2610,15 +2607,15 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C98" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D98" t="s">
-        <v>139</v>
-      </c>
-      <c r="E98" t="s">
+        <v>138</v>
+      </c>
+      <c r="E98">
         <v>1</v>
       </c>
     </row>
@@ -2628,15 +2625,15 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D99" t="s">
-        <v>139</v>
-      </c>
-      <c r="E99" t="s">
+        <v>138</v>
+      </c>
+      <c r="E99">
         <v>1</v>
       </c>
     </row>
@@ -2646,15 +2643,15 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C100" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D100" t="s">
-        <v>139</v>
-      </c>
-      <c r="E100" t="s">
+        <v>138</v>
+      </c>
+      <c r="E100">
         <v>1</v>
       </c>
     </row>
@@ -2664,15 +2661,15 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C101" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D101" t="s">
-        <v>139</v>
-      </c>
-      <c r="E101" t="s">
+        <v>138</v>
+      </c>
+      <c r="E101">
         <v>1</v>
       </c>
     </row>
@@ -2682,15 +2679,15 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C102" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D102" t="s">
-        <v>139</v>
-      </c>
-      <c r="E102" t="s">
+        <v>138</v>
+      </c>
+      <c r="E102">
         <v>1</v>
       </c>
     </row>
@@ -2700,15 +2697,15 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C103" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D103" t="s">
-        <v>139</v>
-      </c>
-      <c r="E103" t="s">
+        <v>138</v>
+      </c>
+      <c r="E103">
         <v>1</v>
       </c>
     </row>
@@ -2718,15 +2715,15 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D104" t="s">
-        <v>139</v>
-      </c>
-      <c r="E104" t="s">
+        <v>138</v>
+      </c>
+      <c r="E104">
         <v>1</v>
       </c>
     </row>
@@ -2736,15 +2733,15 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D105" t="s">
-        <v>139</v>
-      </c>
-      <c r="E105" t="s">
+        <v>138</v>
+      </c>
+      <c r="E105">
         <v>1</v>
       </c>
     </row>
@@ -2754,15 +2751,15 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C106" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D106" t="s">
-        <v>139</v>
-      </c>
-      <c r="E106" t="s">
+        <v>138</v>
+      </c>
+      <c r="E106">
         <v>1</v>
       </c>
     </row>
@@ -2772,15 +2769,15 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C107" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D107" t="s">
-        <v>139</v>
-      </c>
-      <c r="E107" t="s">
+        <v>138</v>
+      </c>
+      <c r="E107">
         <v>1</v>
       </c>
     </row>
@@ -2790,15 +2787,15 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C108" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D108" t="s">
-        <v>139</v>
-      </c>
-      <c r="E108" t="s">
+        <v>138</v>
+      </c>
+      <c r="E108">
         <v>1</v>
       </c>
     </row>
@@ -2808,15 +2805,15 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C109" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D109" t="s">
-        <v>139</v>
-      </c>
-      <c r="E109" t="s">
+        <v>138</v>
+      </c>
+      <c r="E109">
         <v>1</v>
       </c>
     </row>
@@ -2826,15 +2823,15 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C110" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D110" t="s">
-        <v>139</v>
-      </c>
-      <c r="E110" t="s">
+        <v>138</v>
+      </c>
+      <c r="E110">
         <v>1</v>
       </c>
     </row>
@@ -2844,15 +2841,15 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C111" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D111" t="s">
-        <v>139</v>
-      </c>
-      <c r="E111" t="s">
+        <v>138</v>
+      </c>
+      <c r="E111">
         <v>1</v>
       </c>
     </row>
@@ -2862,15 +2859,15 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C112" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D112" t="s">
-        <v>139</v>
-      </c>
-      <c r="E112" t="s">
+        <v>138</v>
+      </c>
+      <c r="E112">
         <v>1</v>
       </c>
     </row>
@@ -2880,15 +2877,15 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C113" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D113" t="s">
-        <v>139</v>
-      </c>
-      <c r="E113" t="s">
+        <v>138</v>
+      </c>
+      <c r="E113">
         <v>1</v>
       </c>
     </row>
@@ -2898,15 +2895,15 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C114" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D114" t="s">
-        <v>139</v>
-      </c>
-      <c r="E114" t="s">
+        <v>138</v>
+      </c>
+      <c r="E114">
         <v>1</v>
       </c>
     </row>
@@ -2916,15 +2913,15 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C115" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D115" t="s">
-        <v>139</v>
-      </c>
-      <c r="E115" t="s">
+        <v>138</v>
+      </c>
+      <c r="E115">
         <v>1</v>
       </c>
     </row>
@@ -2934,15 +2931,15 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C116" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D116" t="s">
-        <v>139</v>
-      </c>
-      <c r="E116" t="s">
+        <v>138</v>
+      </c>
+      <c r="E116">
         <v>1</v>
       </c>
     </row>
@@ -2952,15 +2949,15 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C117" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D117" t="s">
-        <v>139</v>
-      </c>
-      <c r="E117" t="s">
+        <v>138</v>
+      </c>
+      <c r="E117">
         <v>1</v>
       </c>
     </row>
@@ -2970,15 +2967,15 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C118" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D118" t="s">
-        <v>139</v>
-      </c>
-      <c r="E118" t="s">
+        <v>138</v>
+      </c>
+      <c r="E118">
         <v>1</v>
       </c>
     </row>
@@ -2988,15 +2985,15 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C119" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D119" t="s">
-        <v>139</v>
-      </c>
-      <c r="E119" t="s">
+        <v>138</v>
+      </c>
+      <c r="E119">
         <v>1</v>
       </c>
     </row>
@@ -3006,15 +3003,15 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C120" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D120" t="s">
-        <v>139</v>
-      </c>
-      <c r="E120" t="s">
+        <v>138</v>
+      </c>
+      <c r="E120">
         <v>1</v>
       </c>
     </row>
@@ -3024,15 +3021,15 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C121" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D121" t="s">
-        <v>139</v>
-      </c>
-      <c r="E121" t="s">
+        <v>138</v>
+      </c>
+      <c r="E121">
         <v>1</v>
       </c>
     </row>
@@ -3042,15 +3039,15 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C122" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D122" t="s">
-        <v>139</v>
-      </c>
-      <c r="E122" t="s">
+        <v>138</v>
+      </c>
+      <c r="E122">
         <v>1</v>
       </c>
     </row>
@@ -3060,15 +3057,15 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C123" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D123" t="s">
-        <v>139</v>
-      </c>
-      <c r="E123" t="s">
+        <v>138</v>
+      </c>
+      <c r="E123">
         <v>1</v>
       </c>
     </row>
@@ -3078,15 +3075,15 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C124" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D124" t="s">
-        <v>139</v>
-      </c>
-      <c r="E124" t="s">
+        <v>138</v>
+      </c>
+      <c r="E124">
         <v>1</v>
       </c>
     </row>
@@ -3096,15 +3093,15 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C125" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D125" t="s">
-        <v>139</v>
-      </c>
-      <c r="E125" t="s">
+        <v>138</v>
+      </c>
+      <c r="E125">
         <v>1</v>
       </c>
     </row>
@@ -3114,15 +3111,15 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C126" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D126" t="s">
-        <v>139</v>
-      </c>
-      <c r="E126" t="s">
+        <v>138</v>
+      </c>
+      <c r="E126">
         <v>1</v>
       </c>
     </row>
@@ -3132,15 +3129,15 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C127" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D127" t="s">
-        <v>139</v>
-      </c>
-      <c r="E127" t="s">
+        <v>138</v>
+      </c>
+      <c r="E127">
         <v>1</v>
       </c>
     </row>
@@ -3150,15 +3147,15 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C128" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D128" t="s">
-        <v>139</v>
-      </c>
-      <c r="E128" t="s">
+        <v>138</v>
+      </c>
+      <c r="E128">
         <v>1</v>
       </c>
     </row>
@@ -3168,15 +3165,15 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C129" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D129" t="s">
-        <v>139</v>
-      </c>
-      <c r="E129" t="s">
+        <v>138</v>
+      </c>
+      <c r="E129">
         <v>1</v>
       </c>
     </row>
@@ -3186,15 +3183,15 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C130" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D130" t="s">
-        <v>139</v>
-      </c>
-      <c r="E130" t="s">
+        <v>138</v>
+      </c>
+      <c r="E130">
         <v>1</v>
       </c>
     </row>

</xml_diff>